<commit_message>
Indeling learn-python3 eerste opzet
</commit_message>
<xml_diff>
--- a/raw/mogelijke notebooks.xlsx
+++ b/raw/mogelijke notebooks.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32746A3B-9A50-4190-88DE-79DB065F84AF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E7B1BA-40EE-4B8C-9715-6A6D293FE047}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>